<commit_message>
aggiunta salvataggio cg e bt
</commit_message>
<xml_diff>
--- a/F27_truncated/results_f27_3_suplin.xlsx
+++ b/F27_truncated/results_f27_3_suplin.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="224" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="235" uniqueCount="22">
   <si>
     <t>Row</t>
   </si>
@@ -71,6 +71,24 @@
   </si>
   <si>
     <t>n=10^5</t>
+  </si>
+  <si>
+    <t>Average Time</t>
+  </si>
+  <si>
+    <t>Average Iter</t>
+  </si>
+  <si>
+    <t>Violation</t>
+  </si>
+  <si>
+    <t>Average iter Bt</t>
+  </si>
+  <si>
+    <t>Average iter cg</t>
+  </si>
+  <si>
+    <t>N converged</t>
   </si>
 </sst>
 </file>
@@ -212,16 +230,16 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="true"/>
-    <col min="2" max="2" width="13.5546875" customWidth="true"/>
-    <col min="3" max="3" width="12.5546875" customWidth="true"/>
-    <col min="4" max="4" width="9.5546875" customWidth="true"/>
+    <col min="1" max="1" width="13" customWidth="true"/>
+    <col min="2" max="2" width="14.5546875" customWidth="true"/>
+    <col min="3" max="3" width="13.5546875" customWidth="true"/>
+    <col min="4" max="4" width="13.5546875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -240,21 +258,21 @@
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B2" s="0">
-        <v>0.010762027272727273</v>
+        <v>0.021423909090909091</v>
       </c>
       <c r="C2" s="0">
-        <v>0.14205229090909091</v>
+        <v>0.16751673636363631</v>
       </c>
       <c r="D2" s="0">
-        <v>0.80741879999999999</v>
+        <v>1.0377829090909092</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B3" s="0">
         <v>41</v>
@@ -278,6 +296,62 @@
       </c>
       <c r="D4" s="0">
         <v>0.49841515809972309</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="0">
+        <v>0</v>
+      </c>
+      <c r="C5" s="0">
+        <v>0</v>
+      </c>
+      <c r="D5" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="0">
+        <v>0.097560975609756087</v>
+      </c>
+      <c r="C6" s="0">
+        <v>0.042553191489361701</v>
+      </c>
+      <c r="D6" s="0">
+        <v>0.018867924528301886</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="0">
+        <v>1.219512195121951</v>
+      </c>
+      <c r="C7" s="0">
+        <v>1.2127659574468088</v>
+      </c>
+      <c r="D7" s="0">
+        <v>1.1509433962264151</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="0">
+        <v>11</v>
+      </c>
+      <c r="C8" s="0">
+        <v>11</v>
+      </c>
+      <c r="D8" s="0">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>